<commit_message>
refactor purchase and sale report to single function
</commit_message>
<xml_diff>
--- a/report/sale_report_month_2020_01.xlsx
+++ b/report/sale_report_month_2020_01.xlsx
@@ -24,7 +24,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -60,11 +60,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +147,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,10 +171,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.52"/>

</xml_diff>